<commit_message>
updates and corrected final model
</commit_message>
<xml_diff>
--- a/BPA/Ch.10/model descriptions.xlsx
+++ b/BPA/Ch.10/model descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/thomas_buehrens_dfw_wa_gov/Documents/Documents/Scripts/stan_example-models/BPA/Ch.10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_F25DC773A252ABDACC104847B9996F945BDE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F03FA15-25AD-4A79-B486-6EF281C33D14}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_F25DC773A252ABDACC104847B9996F945BDE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B2F317F-39AD-456E-9C90-27AECCDA7240}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
   <si>
     <t>js_super_indran</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>length effect on p</t>
+  </si>
+  <si>
+    <t>js_super_indran_thomas_space_time_length</t>
+  </si>
+  <si>
+    <t>variable period length</t>
   </si>
 </sst>
 </file>
@@ -94,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -419,10 +432,11 @@
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="11" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -448,13 +462,16 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,7 +479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -478,65 +495,106 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix r script to run models
</commit_message>
<xml_diff>
--- a/BPA/Ch.10/model descriptions.xlsx
+++ b/BPA/Ch.10/model descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/thomas_buehrens_dfw_wa_gov/Documents/Documents/Scripts/stan_example-models/BPA/Ch.10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC104847B9996F945BDE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D276901-4EA7-4092-AA6C-0D7206510126}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_F25DC773A252ABDACC104847B9996F945BDE58FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CB1314C-379A-470F-B64B-6EFE4B88D80C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <t>variable period length</t>
   </si>
   <si>
-    <t>sorta…close but…hmmm</t>
-  </si>
-  <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>pretty darn good…I think so</t>
   </si>
 </sst>
 </file>
@@ -109,18 +109,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -153,12 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +435,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,76 +511,76 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>19</v>
+      <c r="J3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -614,11 +607,11 @@
       <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>20</v>
+      <c r="J6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>